<commit_message>
- Update - Performance
</commit_message>
<xml_diff>
--- a/Data/Portfolio sorting/Data_5_Factors_2x3_daily.xlsx
+++ b/Data/Portfolio sorting/Data_5_Factors_2x3_daily.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Panagiotis.Mavritsak\Desktop\Reddit sentiment analysis\Part2\part 2 data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://deltares-my.sharepoint.com/personal/antonis_mavritsakis_deltares_nl/Documents/Documents/Python Projects/wsb-sentiment-analysis/Data/Portfolio sorting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F635390-19B9-4D08-A69D-7F09445EA9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{8F635390-19B9-4D08-A69D-7F09445EA9C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC2A91F8-6CFF-4BEA-B8DA-41607BEE579B}"/>
   <bookViews>
-    <workbookView xWindow="74562" yWindow="3600" windowWidth="21600" windowHeight="12318"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_5_Factors_2x3_daily" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -46,7 +56,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -880,14 +890,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G252"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="B253" sqref="B253"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -910,7 +922,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20210105</v>
       </c>
@@ -933,7 +945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>20210106</v>
       </c>
@@ -956,7 +968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>20210107</v>
       </c>
@@ -979,7 +991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>20210108</v>
       </c>
@@ -1002,7 +1014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>20210111</v>
       </c>
@@ -1025,7 +1037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>20210112</v>
       </c>
@@ -1048,7 +1060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>20210113</v>
       </c>
@@ -1071,7 +1083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>20210114</v>
       </c>
@@ -1094,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>20210115</v>
       </c>
@@ -1117,7 +1129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>20210119</v>
       </c>
@@ -1140,7 +1152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>20210120</v>
       </c>
@@ -1163,7 +1175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>20210121</v>
       </c>
@@ -1186,7 +1198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>20210122</v>
       </c>
@@ -1209,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>20210125</v>
       </c>
@@ -1232,7 +1244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>20210126</v>
       </c>
@@ -1255,7 +1267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>20210127</v>
       </c>
@@ -1278,7 +1290,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>20210128</v>
       </c>
@@ -1301,7 +1313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>20210129</v>
       </c>
@@ -1324,7 +1336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>20210201</v>
       </c>
@@ -1347,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20210202</v>
       </c>
@@ -1370,7 +1382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20210203</v>
       </c>
@@ -1393,7 +1405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>20210204</v>
       </c>
@@ -1416,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>20210205</v>
       </c>
@@ -1439,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>20210208</v>
       </c>
@@ -1462,7 +1474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>20210209</v>
       </c>
@@ -1485,7 +1497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>20210210</v>
       </c>
@@ -1508,7 +1520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>20210211</v>
       </c>
@@ -1531,7 +1543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>20210212</v>
       </c>
@@ -1554,7 +1566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>20210216</v>
       </c>
@@ -1577,7 +1589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>20210217</v>
       </c>
@@ -1600,7 +1612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>20210218</v>
       </c>
@@ -1623,7 +1635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>20210219</v>
       </c>
@@ -1646,7 +1658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>20210222</v>
       </c>
@@ -1669,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>20210223</v>
       </c>
@@ -1692,7 +1704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>20210224</v>
       </c>
@@ -1715,7 +1727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>20210225</v>
       </c>
@@ -1738,7 +1750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>20210226</v>
       </c>
@@ -1761,7 +1773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>20210301</v>
       </c>
@@ -1784,7 +1796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>20210302</v>
       </c>
@@ -1807,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>20210303</v>
       </c>
@@ -1830,7 +1842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>20210304</v>
       </c>
@@ -1853,7 +1865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>20210305</v>
       </c>
@@ -1876,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>20210308</v>
       </c>
@@ -1899,7 +1911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>20210309</v>
       </c>
@@ -1922,7 +1934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>20210310</v>
       </c>
@@ -1945,7 +1957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>20210311</v>
       </c>
@@ -1968,7 +1980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>20210312</v>
       </c>
@@ -1991,7 +2003,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>20210315</v>
       </c>
@@ -2014,7 +2026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>20210316</v>
       </c>
@@ -2037,7 +2049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>20210317</v>
       </c>
@@ -2060,7 +2072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>20210318</v>
       </c>
@@ -2083,7 +2095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>20210319</v>
       </c>
@@ -2106,7 +2118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>20210322</v>
       </c>
@@ -2129,7 +2141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>20210323</v>
       </c>
@@ -2152,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>20210324</v>
       </c>
@@ -2175,7 +2187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>20210325</v>
       </c>
@@ -2198,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>20210326</v>
       </c>
@@ -2221,7 +2233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>20210329</v>
       </c>
@@ -2244,7 +2256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>20210330</v>
       </c>
@@ -2267,7 +2279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>20210331</v>
       </c>
@@ -2290,7 +2302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>20210401</v>
       </c>
@@ -2313,7 +2325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>20210405</v>
       </c>
@@ -2336,7 +2348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>20210406</v>
       </c>
@@ -2359,7 +2371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>20210407</v>
       </c>
@@ -2382,7 +2394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>20210408</v>
       </c>
@@ -2405,7 +2417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>20210409</v>
       </c>
@@ -2428,7 +2440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>20210412</v>
       </c>
@@ -2451,7 +2463,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>20210413</v>
       </c>
@@ -2474,7 +2486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>20210414</v>
       </c>
@@ -2497,7 +2509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>20210415</v>
       </c>
@@ -2520,7 +2532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>20210416</v>
       </c>
@@ -2543,7 +2555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>20210419</v>
       </c>
@@ -2566,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>20210420</v>
       </c>
@@ -2589,7 +2601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>20210421</v>
       </c>
@@ -2612,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>20210422</v>
       </c>
@@ -2635,7 +2647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>20210423</v>
       </c>
@@ -2658,7 +2670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>20210426</v>
       </c>
@@ -2681,7 +2693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>20210427</v>
       </c>
@@ -2704,7 +2716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>20210428</v>
       </c>
@@ -2727,7 +2739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>20210429</v>
       </c>
@@ -2750,7 +2762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>20210430</v>
       </c>
@@ -2773,7 +2785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>20210503</v>
       </c>
@@ -2796,7 +2808,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>20210504</v>
       </c>
@@ -2819,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>20210505</v>
       </c>
@@ -2842,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>20210506</v>
       </c>
@@ -2865,7 +2877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>20210507</v>
       </c>
@@ -2888,7 +2900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>20210510</v>
       </c>
@@ -2911,7 +2923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>20210511</v>
       </c>
@@ -2934,7 +2946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>20210512</v>
       </c>
@@ -2957,7 +2969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>20210513</v>
       </c>
@@ -2980,7 +2992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>20210514</v>
       </c>
@@ -3003,7 +3015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>20210517</v>
       </c>
@@ -3026,7 +3038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>20210518</v>
       </c>
@@ -3049,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>20210519</v>
       </c>
@@ -3072,7 +3084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>20210520</v>
       </c>
@@ -3095,7 +3107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>20210521</v>
       </c>
@@ -3118,7 +3130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>20210524</v>
       </c>
@@ -3141,7 +3153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>20210525</v>
       </c>
@@ -3164,7 +3176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>20210526</v>
       </c>
@@ -3187,7 +3199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>20210527</v>
       </c>
@@ -3210,7 +3222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>20210528</v>
       </c>
@@ -3233,7 +3245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>20210601</v>
       </c>
@@ -3256,7 +3268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>20210602</v>
       </c>
@@ -3279,7 +3291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>20210603</v>
       </c>
@@ -3302,7 +3314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>20210604</v>
       </c>
@@ -3325,7 +3337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>20210607</v>
       </c>
@@ -3348,7 +3360,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>20210608</v>
       </c>
@@ -3371,7 +3383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>20210609</v>
       </c>
@@ -3394,7 +3406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>20210610</v>
       </c>
@@ -3417,7 +3429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>20210611</v>
       </c>
@@ -3440,7 +3452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>20210614</v>
       </c>
@@ -3463,7 +3475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>20210615</v>
       </c>
@@ -3486,7 +3498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>20210616</v>
       </c>
@@ -3509,7 +3521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>20210617</v>
       </c>
@@ -3532,7 +3544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>20210618</v>
       </c>
@@ -3555,7 +3567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>20210621</v>
       </c>
@@ -3578,7 +3590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>20210622</v>
       </c>
@@ -3601,7 +3613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>20210623</v>
       </c>
@@ -3624,7 +3636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>20210624</v>
       </c>
@@ -3647,7 +3659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>20210625</v>
       </c>
@@ -3670,7 +3682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>20210628</v>
       </c>
@@ -3693,7 +3705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>20210629</v>
       </c>
@@ -3716,7 +3728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>20210630</v>
       </c>
@@ -3739,7 +3751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>20210701</v>
       </c>
@@ -3762,7 +3774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>20210702</v>
       </c>
@@ -3785,7 +3797,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>20210706</v>
       </c>
@@ -3808,7 +3820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>20210707</v>
       </c>
@@ -3831,7 +3843,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>20210708</v>
       </c>
@@ -3854,7 +3866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>20210709</v>
       </c>
@@ -3877,7 +3889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>20210712</v>
       </c>
@@ -3900,7 +3912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>20210713</v>
       </c>
@@ -3923,7 +3935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>20210714</v>
       </c>
@@ -3946,7 +3958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>20210715</v>
       </c>
@@ -3969,7 +3981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>20210716</v>
       </c>
@@ -3992,7 +4004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>20210719</v>
       </c>
@@ -4015,7 +4027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>20210720</v>
       </c>
@@ -4038,7 +4050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>20210721</v>
       </c>
@@ -4061,7 +4073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>20210722</v>
       </c>
@@ -4084,7 +4096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>20210723</v>
       </c>
@@ -4107,7 +4119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>20210726</v>
       </c>
@@ -4130,7 +4142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>20210727</v>
       </c>
@@ -4153,7 +4165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>20210728</v>
       </c>
@@ -4176,7 +4188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>20210729</v>
       </c>
@@ -4199,7 +4211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>20210730</v>
       </c>
@@ -4222,7 +4234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>20210802</v>
       </c>
@@ -4245,7 +4257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>20210803</v>
       </c>
@@ -4268,7 +4280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>20210804</v>
       </c>
@@ -4291,7 +4303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>20210805</v>
       </c>
@@ -4314,7 +4326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>20210806</v>
       </c>
@@ -4337,7 +4349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>20210809</v>
       </c>
@@ -4360,7 +4372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>20210810</v>
       </c>
@@ -4383,7 +4395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>20210811</v>
       </c>
@@ -4406,7 +4418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>20210812</v>
       </c>
@@ -4429,7 +4441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>20210813</v>
       </c>
@@ -4452,7 +4464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>20210816</v>
       </c>
@@ -4475,7 +4487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>20210817</v>
       </c>
@@ -4498,7 +4510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>20210818</v>
       </c>
@@ -4521,7 +4533,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>20210819</v>
       </c>
@@ -4544,7 +4556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>20210820</v>
       </c>
@@ -4567,7 +4579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>20210823</v>
       </c>
@@ -4590,7 +4602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>20210824</v>
       </c>
@@ -4613,7 +4625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>20210825</v>
       </c>
@@ -4636,7 +4648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>20210826</v>
       </c>
@@ -4659,7 +4671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>20210827</v>
       </c>
@@ -4682,7 +4694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>20210830</v>
       </c>
@@ -4705,7 +4717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>20210831</v>
       </c>
@@ -4728,7 +4740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>20210901</v>
       </c>
@@ -4751,7 +4763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>20210902</v>
       </c>
@@ -4774,7 +4786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>20210903</v>
       </c>
@@ -4797,7 +4809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>20210907</v>
       </c>
@@ -4820,7 +4832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>20210908</v>
       </c>
@@ -4843,7 +4855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>20210909</v>
       </c>
@@ -4866,7 +4878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>20210910</v>
       </c>
@@ -4889,7 +4901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>20210913</v>
       </c>
@@ -4912,7 +4924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>20210914</v>
       </c>
@@ -4935,7 +4947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>20210915</v>
       </c>
@@ -4958,7 +4970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>20210916</v>
       </c>
@@ -4981,7 +4993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>20210917</v>
       </c>
@@ -5004,7 +5016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>20210920</v>
       </c>
@@ -5027,7 +5039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>20210921</v>
       </c>
@@ -5050,7 +5062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>20210922</v>
       </c>
@@ -5073,7 +5085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>20210923</v>
       </c>
@@ -5096,7 +5108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>20210924</v>
       </c>
@@ -5119,7 +5131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>20210927</v>
       </c>
@@ -5142,7 +5154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>20210928</v>
       </c>
@@ -5165,7 +5177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>20210929</v>
       </c>
@@ -5188,7 +5200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>20210930</v>
       </c>
@@ -5211,7 +5223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>20211001</v>
       </c>
@@ -5234,7 +5246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>20211004</v>
       </c>
@@ -5257,7 +5269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>20211005</v>
       </c>
@@ -5280,7 +5292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>20211006</v>
       </c>
@@ -5303,7 +5315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>20211007</v>
       </c>
@@ -5326,7 +5338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>20211008</v>
       </c>
@@ -5349,7 +5361,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>20211011</v>
       </c>
@@ -5372,7 +5384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>20211012</v>
       </c>
@@ -5395,7 +5407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>20211013</v>
       </c>
@@ -5418,7 +5430,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>20211014</v>
       </c>
@@ -5441,7 +5453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>20211015</v>
       </c>
@@ -5464,7 +5476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>20211018</v>
       </c>
@@ -5487,7 +5499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>20211019</v>
       </c>
@@ -5510,7 +5522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>20211020</v>
       </c>
@@ -5533,7 +5545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>20211021</v>
       </c>
@@ -5556,7 +5568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>20211022</v>
       </c>
@@ -5579,7 +5591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>20211025</v>
       </c>
@@ -5602,7 +5614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>20211026</v>
       </c>
@@ -5625,7 +5637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>20211027</v>
       </c>
@@ -5648,7 +5660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>20211028</v>
       </c>
@@ -5671,7 +5683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>20211029</v>
       </c>
@@ -5694,7 +5706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>20211101</v>
       </c>
@@ -5717,7 +5729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>20211102</v>
       </c>
@@ -5740,7 +5752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>20211103</v>
       </c>
@@ -5763,7 +5775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>20211104</v>
       </c>
@@ -5786,7 +5798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>20211105</v>
       </c>
@@ -5809,7 +5821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>20211108</v>
       </c>
@@ -5832,7 +5844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>20211109</v>
       </c>
@@ -5855,7 +5867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>20211110</v>
       </c>
@@ -5878,7 +5890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>20211111</v>
       </c>
@@ -5901,7 +5913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>20211112</v>
       </c>
@@ -5924,7 +5936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>20211115</v>
       </c>
@@ -5947,7 +5959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>20211116</v>
       </c>
@@ -5970,7 +5982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>20211117</v>
       </c>
@@ -5993,7 +6005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>20211118</v>
       </c>
@@ -6016,7 +6028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>20211119</v>
       </c>
@@ -6039,7 +6051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>20211122</v>
       </c>
@@ -6062,7 +6074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>20211123</v>
       </c>
@@ -6085,7 +6097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>20211124</v>
       </c>
@@ -6108,7 +6120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>20211126</v>
       </c>
@@ -6131,7 +6143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>20211129</v>
       </c>
@@ -6154,7 +6166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>20211130</v>
       </c>
@@ -6177,7 +6189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>20211201</v>
       </c>
@@ -6200,7 +6212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>20211202</v>
       </c>
@@ -6223,7 +6235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>20211203</v>
       </c>
@@ -6246,7 +6258,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>20211206</v>
       </c>
@@ -6269,7 +6281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>20211207</v>
       </c>
@@ -6292,7 +6304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>20211208</v>
       </c>
@@ -6315,7 +6327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>20211209</v>
       </c>
@@ -6338,7 +6350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>20211210</v>
       </c>
@@ -6361,7 +6373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>20211213</v>
       </c>
@@ -6384,7 +6396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>20211214</v>
       </c>
@@ -6407,7 +6419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>20211215</v>
       </c>
@@ -6430,7 +6442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>20211216</v>
       </c>
@@ -6453,7 +6465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>20211217</v>
       </c>
@@ -6476,7 +6488,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>20211220</v>
       </c>
@@ -6499,7 +6511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>20211221</v>
       </c>
@@ -6522,7 +6534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>20211222</v>
       </c>
@@ -6545,7 +6557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>20211223</v>
       </c>
@@ -6568,7 +6580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>20211227</v>
       </c>
@@ -6591,7 +6603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>20211228</v>
       </c>
@@ -6614,7 +6626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>20211229</v>
       </c>
@@ -6637,7 +6649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>20211230</v>
       </c>
@@ -6660,7 +6672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>20211231</v>
       </c>
@@ -6681,6 +6693,12 @@
       </c>
       <c r="G252">
         <v>0</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B253">
+        <f>SUM(B223:B252)</f>
+        <v>5.2699999999999987</v>
       </c>
     </row>
   </sheetData>

</xml_diff>